<commit_message>
se agrega la funcion para exportacion reseña a word con un archivo separado
</commit_message>
<xml_diff>
--- a/contenido_archivos.xlsx
+++ b/contenido_archivos.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -478,190 +478,190 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>/Users/alexisjankowicz/Python/pdf_a_excel/BALVANERA96 -DOS (02) DETENIDOS.pdf</t>
+          <t>/Users/alexisjankowicz/Python/pdf_a_excel/PARTE SUCESO 45688136.pdf</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>22 de Julio de 2025</t>
+          <t>22 de julio del 2025</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>01:55</t>
+          <t>09:15</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>TTVA ROBO</t>
+          <t>HURTO MOTOVEHICULAR</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Inspector ARGUELLO Leandro</t>
+          <t>Oficial Mayor MARTÍNEZ, Ricardo</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Of QUINTANA Gilda</t>
+          <t>Inspector NIEVA, Juan</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Cont INFANTE Jonathan</t>
+          <t>Pers, Contratado ORDEÑEZ, Débora.</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>DOS (02) DETENIDOS</t>
+          <t>TRES (03) DETENIDOS</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>/Users/alexisjankowicz/Python/pdf_a_excel/BALVANERA96 -DOS (02) DETENIDOS.pdf</t>
+          <t>/Users/alexisjankowicz/Python/pdf_a_excel/PARTE SUCESO 45688962.pdf</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>22 de Julio de 2025</t>
+          <t>22 de julio del 2025</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>01:55</t>
+          <t>12:45</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>TTVA ROBO</t>
+          <t>S/D</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Inspector ARGUELLO Leandro</t>
+          <t>Oficial Mayor MARTÍNEZ, Ricardo</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Of QUINTANA Gilda</t>
+          <t>Oficial GUZMAN, Yesica</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Cont INFANTE Jonathan</t>
+          <t>Pers, Contratado BARONE, Candela.</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>DOS (02) DETENIDOS</t>
+          <t>UN (01) DETENIDO</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>/Users/alexisjankowicz/Python/pdf_a_excel/RETIRO55 - UN (01) DETENIDO.pdf</t>
+          <t>/Users/alexisjankowicz/Python/pdf_a_excel/PARTE_SUCESO_45705933.pdf</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>22 de Julio de 2025</t>
+          <t>24 de julio del 2025</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>01:53</t>
+          <t>16:50</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>TTVA ROBO</t>
+          <t>Infracción Ley 23737</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Inspector ARGUELLO Leandro</t>
+          <t>Of. Mayor MARTINEZ, Ricardo</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Of Primero VILLALBA Nicolas</t>
+          <t>Of Mayor MEZA, Gastón</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Cont BENITEZ PEREIRA Patricia</t>
+          <t>Pers. Contratado TURA, Belén</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>DOS (02) DETENIDOS</t>
+          <t>UN (01) DETENIDO</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>/Users/alexisjankowicz/Python/pdf_a_excel/PARTE SUCESO 45688136.pdf</t>
+          <t>/Users/alexisjankowicz/Python/pdf_a_excel/BALVANERA96 -DOS (02) DETENIDOS.pdf</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>22 de julio del 2025</t>
+          <t>22 de Julio de 2025</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>09:15</t>
+          <t>01:55</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>HURTO MOTOVEHICULAR</t>
+          <t>TTVA ROBO</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Oficial Mayor MARTÍNEZ, Ricardo</t>
+          <t>Inspector ARGUELLO Leandro</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Inspector NIEVA, Juan</t>
+          <t>Of QUINTANA Gilda</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Pers, Contratado ORDEÑEZ, Débora.</t>
+          <t>Cont INFANTE Jonathan</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>TRES (03) DETENIDOS</t>
+          <t>DOS (02) DETENIDOS</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>/Users/alexisjankowicz/Python/pdf_a_excel/CONSTITUCIÓN74 - DOS (02) DETENIDOS.pdf</t>
+          <t>/Users/alexisjankowicz/Python/pdf_a_excel/RETIRO55 - UN (01) DETENIDO.pdf</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>24 de Julio de 2025</t>
+          <t>22 de Julio de 2025</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>16:32</t>
+          <t>01:53</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>LEY 23737</t>
+          <t>TTVA ROBO</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -671,17 +671,59 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Of Mayor MEZA Gastón</t>
+          <t>Of Primero VILLALBA Nicolas</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Cont LEGUINA Daniel</t>
+          <t>Cont BENITEZ PEREIRA Patricia</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
           <t>DOS (02) DETENIDOS</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>/Users/alexisjankowicz/Python/pdf_a_excel/PARTE SUCESO 45688136.pdf</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>22 de julio del 2025</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>09:15</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>HURTO MOTOVEHICULAR</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Oficial Mayor MARTÍNEZ, Ricardo</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Inspector NIEVA, Juan</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Pers, Contratado ORDEÑEZ, Débora.</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>TRES (03) DETENIDOS</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualizacion de archivo funcional a V2.2; borrado de archivo previo y desechables
</commit_message>
<xml_diff>
--- a/contenido_archivos.xlsx
+++ b/contenido_archivos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:I40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,20 +456,25 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
+          <t>sae</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
           <t>jefe de servicio</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>oficial de servicio</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>operador de camara</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>resultado</t>
         </is>
@@ -478,252 +483,1833 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>/Users/alexisjankowicz/Python/pdf_a_excel/PARTE SUCESO 45688136.pdf</t>
+          <t>/Volumes/SIN NOMBRE/ultimo casi/PARTES/(01) CONTRAVENTOR SAN NICOLÁS 57.pdf</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>22 de julio del 2025</t>
+          <t>24/08/2025</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>09:15</t>
+          <t>21:14</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>HURTO MOTOVEHICULAR</t>
+          <t>“Cuida coches”</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Oficial Mayor MARTÍNEZ, Ricardo</t>
+          <t>45939263</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Inspector NIEVA, Juan</t>
+          <t>INSPECTOR Kelly, Aileen. -</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Pers, Contratado ORDEÑEZ, Débora.</t>
+          <t>OFICIAL Beñacar, Silvina. -</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>TRES (03) DETENIDOS</t>
+          <t>PERSONAL CONTRATADO Monzalvo, Sofía. -</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>UN (01) CONTRAVENTOR. –</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>/Users/alexisjankowicz/Python/pdf_a_excel/PARTE SUCESO 45688962.pdf</t>
+          <t>/Volumes/SIN NOMBRE/ultimo casi/PARTES/(01) DETENIDO CONSTITUCIÓN 32 - CONSTITUCIÓN 85.pdf</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>22 de julio del 2025</t>
+          <t>25/08/2025</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>12:45</t>
+          <t>00:29</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>S/D</t>
+          <t>“Tentativa de Hurto”</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Oficial Mayor MARTÍNEZ, Ricardo</t>
+          <t>45940239</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Oficial GUZMAN, Yesica</t>
+          <t>INSPECTOR Kelly, Aileen. -</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Pers, Contratado BARONE, Candela.</t>
+          <t>OFICIAL Beñacar, Silvina. -</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>UN (01) DETENIDO</t>
+          <t>PERSONAL CONTRATADO Aquino, Juliana. -</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>UN (01)</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>/Users/alexisjankowicz/Python/pdf_a_excel/PARTE_SUCESO_45705933.pdf</t>
+          <t>/Volumes/SIN NOMBRE/ultimo casi/PARTES/(01) DETENIDO SAAVEDRA 46 CAM02.pdf</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>24 de julio del 2025</t>
+          <t>24/08/2025</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>16:50</t>
+          <t>20:41</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Infracción Ley 23737</t>
+          <t>“Tentativa de Hurto”</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Of. Mayor MARTINEZ, Ricardo</t>
+          <t>45939052</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Of Mayor MEZA, Gastón</t>
+          <t>INSPECTOR Kelly, Aileen. -</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Pers. Contratado TURA, Belén</t>
+          <t>OFICIAL MAYOR Benítez, Antonella. -</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>UN (01) DETENIDO</t>
+          <t>PERSONAL CONTRATADO Gavello, Anabella. -</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>UN (01) DETENIDO. –</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>/Users/alexisjankowicz/Python/pdf_a_excel/BALVANERA96 -DOS (02) DETENIDOS.pdf</t>
+          <t>/Volumes/SIN NOMBRE/ultimo casi/PARTES/(01) DETENIDO VILLA LUGANO O110 - VILLA LUGANO O133 CAM02- VILLA LUGANO 21.pdf</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>22 de Julio de 2025</t>
+          <t>25/08/2025</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>01:55</t>
+          <t>05:24</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>TTVA ROBO</t>
+          <t>“Incendio”</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Inspector ARGUELLO Leandro</t>
+          <t>45940965</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Of QUINTANA Gilda</t>
+          <t>INSPECTOR Kelly, Aileen. -</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Cont INFANTE Jonathan</t>
+          <t>OFICIAL MAYOR González, Elizabeth. -</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>DOS (02) DETENIDOS</t>
+          <t>PERSONAL CONTRATADO Carrera, Débora. -</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>UN</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>/Users/alexisjankowicz/Python/pdf_a_excel/RETIRO55 - UN (01) DETENIDO.pdf</t>
+          <t>/Volumes/SIN NOMBRE/ultimo casi/PARTES/(01) IMPUTADO PUERTO MADERO 03.pdf</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>22 de Julio de 2025</t>
+          <t>25/08/2025</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>01:53</t>
+          <t>01:51</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>TTVA ROBO</t>
+          <t>“Maltrato”</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Inspector ARGUELLO Leandro</t>
+          <t>45940514</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Of Primero VILLALBA Nicolas</t>
+          <t>INSPECTOR Kelly, Aileen. -</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Cont BENITEZ PEREIRA Patricia</t>
+          <t>OFICIAL Rodríguez, Fernando. -</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>DOS (02) DETENIDOS</t>
+          <t>AUXILIAR Garrigo, Agustina. -</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>UN (01) IMPUTADO. –</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>/Users/alexisjankowicz/Python/pdf_a_excel/PARTE SUCESO 45688136.pdf</t>
+          <t>/Volumes/SIN NOMBRE/ultimo casi/PARTES/(02) DETENIDOS BOCA 60 - BOCA 25.pdf</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>22 de julio del 2025</t>
+          <t>24/08/2025</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>09:15</t>
+          <t>19:34</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>HURTO MOTOVEHICULAR</t>
+          <t>“Robo”</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Oficial Mayor MARTÍNEZ, Ricardo</t>
+          <t>45938679</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Inspector NIEVA, Juan</t>
+          <t>INSPECTOR Kelly, Aileen. -</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Pers, Contratado ORDEÑEZ, Débora.</t>
+          <t>OFICIAL Rodríguez, Fernando. -</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>TRES (03) DETENIDOS</t>
+          <t>PERSONAL CONTRATADO Prezzavento, Sergio. -</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>DOS (02) DETENIDOS. –</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>/Volumes/SIN NOMBRE/ultimo casi/PARTES/(02) DETENIDOS CONSTITUCIÓN 13.pdf</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>25/08/2025</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>01:10</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>“Amenazas”</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>45940409</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>INSPECTOR Kelly, Aileen. -</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>OFICIAL Beñacar, Silvina. -</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>PERSONAL CONTRATADO Zoraire, Micaela. -</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>UN (01)</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>/Volumes/SIN NOMBRE/ultimo casi/PARTES/01 CONTRAVENTOR -CUIDACOCHES-FLORESTA44.docx (1).pdf</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>26  de  agosto  de  2025</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>14:20</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Cuidacoches</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>45950775</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Inspector  LP  4532  Aguirre  Alan</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Oficial  LP  37722  Bustamante  Lis</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>Pers  Contratado  Cardozo  Romina</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>UN  (01)  CONTRAVENTOR</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>/Volumes/SIN NOMBRE/ultimo casi/PARTES/01 CONTRAVENTOR -CUIDACOCHES-FLORESTA44.docx.pdf</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>26  de  agosto  de  2025</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>10:50</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Cuidacoches</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>45949355</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Inspector  LP  4532  Aguirre  Alan</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Oficial  LP  37722  Bustamante,  Lis</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>Pers.  Contratado  Cardozo  Romina</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>UN  (01)  CONTRAVENTOR</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>/Volumes/SIN NOMBRE/ultimo casi/PARTES/01 CONTRAVENTOR -USO INDEBIDO DE ESPACIO PUBLICO-ALMAGRO23.docx.pdf</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>26  de  agosto  de  2025</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>14:05</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Uso  indebido  de  espacio  público</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>45950364</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Inspector  LP  4532  Aguirre  Alan</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Oficial  LP  37722  Bustamante  Lis</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>Auxiliar  Penovi  Lucas</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>UN  (01)  CONTRAVENTOR</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>/Volumes/SIN NOMBRE/ultimo casi/PARTES/01 DETENIDO - RESITENCIA _AMENAZAS - FLORES 29 .docx (1).pdf</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>26  de  Agosto  del  2025</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>05:23hs.-</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Resistencia  y  Amenazas</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>45948526</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Inspector  CISNEROS,  Pablo.  -</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>Oficial  Mayor  LANGE  Daniel</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>Meza  Romina</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>UN  (01)  DETENIDO  .  -</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>/Volumes/SIN NOMBRE/ultimo casi/PARTES/01 DETENIDO - ROBO - FLORES 69.pdf</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>25 de agosto de 2025</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>20:15 Hs.-</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Actuaciones por Robo</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>45945683</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Inspector  Cisneros, Pablo. -</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Inspector Leiva, Jorge</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>PC Almeda, Micaela.</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>UN (01) DETENIDO. -</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>/Volumes/SIN NOMBRE/ultimo casi/PARTES/1 DETENIDO- 45944647.pdf</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>25 de Agosto del 2025</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>17:04</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>DAÑOS</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>45944647</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Oficial Mayor VERA, Erika.</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>Oficial Primero PEREZ, Ramón</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>S/D</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>UN (01) DETENIDO</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>/Volumes/SIN NOMBRE/ultimo casi/PARTES/1 DETENIDO- SAE 45941801.pdf</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>25 de Agosto del 2025</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>10:18</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>ROBO</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>45941801</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Oficial Mayor VERA, Erika.</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>Oficial BUSTAMANTE, Lis.</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>S/D</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>UN (01) DETENIDO</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>/Volumes/SIN NOMBRE/ultimo casi/PARTES/1 DETENIDO- SAE 45943591.pdf</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>25 de Agosto del 2025</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>15:20</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Autor detenido por particulares</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>45943591</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Oficial Mayor VERA, Erika.</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>Oficial BUSTAMANTE, Lis.</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>S/D</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>UN (01) DETENIDO</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>/Volumes/SIN NOMBRE/ultimo casi/PARTES/1 DETENIDO- SAE 45943869.pdf</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>25 de Agosto del 2025</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>16:40</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>ART 239 Y 89</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>45943869</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Oficial Mayor VERA, Erika.</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>Oficial Primero PEREZ, Ramon</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>S/D</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>UN (01) DETENIDO</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>/Volumes/SIN NOMBRE/ultimo casi/PARTES/1 DETENIDO- SAE 45943917.pdf</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>25 de Agosto del 2025</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>16:01</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>ROBO</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>45943917</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Oficial Mayor VERA, Erika.</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>Inspector NIEVA, Juan.</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>S/D</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>UN (01) DETENIDO</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>/Volumes/SIN NOMBRE/ultimo casi/PARTES/01 DETENIDO-TTVA ROBO-CONSTITUCION 20 .docx.pdf</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>26  de  agosto  de  2025</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>16:47</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Robo</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>45951575</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Inspector  LP  4532  Aguirre  Alan</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>Oficial  lp  34696   Arellano  Federico  34696</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>Personal  Contratado  Castillo  Gisell</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>UN    (01)  DETENIDO</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>/Volumes/SIN NOMBRE/ultimo casi/PARTES/01 DETENIDO-TTVA ROBO-POMPEYA 90.docx.pdf</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>26  de  agosto  de  2025</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>14:43</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Robo</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>45950070</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Inspector  LP  4532  Aguirre  Alan</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>Oficial  LP29249   Guzman  Yesica</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>Personal  Contratado  Silva  Vanesa</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>UN    (01)  DETENIDO</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>/Volumes/SIN NOMBRE/ultimo casi/PARTES/01 IMPUTADO -ART 91 _ ART 239- FLORESTA50.docx.pdf</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>26  de  agosto  de  2025</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>11:08</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Art  91/art  239</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>45949837</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Inspector  LP  4532  Aguirre  Alan</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>Oficial  LP  37722  Bustamante,  Lis</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>Auxiliar  Soldani  Clara</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>UN  (01)  IMPUTADO</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>/Volumes/SIN NOMBRE/ultimo casi/PARTES/01 IMPUTADO -ART 133- nuñezo125.docx.pdf</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>26  de  agosto  de  2025</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>12:55</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Art  133</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>45949872</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>Inspector  LP  4532  Aguirre  Alan</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>Oficial  Primero  LP  6221  Oropeza  Mauro</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>Personal  Contratado  Karchacoff  Nahir</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>UN  (01)  IMPUTADO</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>/Volumes/SIN NOMBRE/ultimo casi/PARTES/01 IMPUTADO -LESIONES 94-CONSTITUCION 07 .docx.pdf</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>26  de  agosto  de  2025</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>14:08</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Lesiones  94</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>45949421</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>Inspector  LP  4532  Aguirre  Alan</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>Oficial  LP29249   Guzman  Yesica</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>Auxiliar  Gomez  Valeria</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>UN    (01)  IMPUTADO</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>/Volumes/SIN NOMBRE/ultimo casi/PARTES/1 IMPUTADO- SAE 45957587.pdf</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>27 de Agosto del 2025</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>11:30</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Articulo 103</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>45957587</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>Oficial Mayor VERA, Erika.</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>Oficial GAUNA, Micaela.</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>S/D</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>UN (01) CONTRAVENTOR</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>/Volumes/SIN NOMBRE/ultimo casi/PARTES/01 IMPUTADO-ART91- PALERMO207.docx.pdf</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>25  de  Agosto  del  2025</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>21:00  hs.-</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Art.  91</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>45946280</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>Inspector  CISNEROS,  Pablo.  -</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>Oficial  Mayor  LANGE  Daniel</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>ARGAÑARAZ  Brian</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>UN  (01)  IMPUTADO.  -</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>/Volumes/SIN NOMBRE/ultimo casi/PARTES/01 IMPUTADO-ARTICULO54- RECOLETA47.docx.pdf</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>26  de  Agosto  del  2025</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>00:34  hs.-</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>artículo  54</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>45946977</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>Inspector  CISNEROS,  Pablo.  -</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>Oficial  Primero  CARABAJAL  Mariana</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>ALEGRE  Emilce</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>UN  (01)  IMPUTADO.  -</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>/Volumes/SIN NOMBRE/ultimo casi/PARTES/01 IMPUTADO-LEY 23737 ART29Y30- CONSTITUCION74.docx.pdf</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>25  de  Agosto  del  2025</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>22:54  hs.-</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Ley  23737,  Art  29  y  30</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>45947241</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>Inspector  CISNEROS,  Pablo.  -</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>Oficial  Primero  RIVERO  Marcos.-</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>YUFRA  Yohana</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>UN  (01)  IMPUTADO.  -</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>/Volumes/SIN NOMBRE/ultimo casi/PARTES/01DETENIDO-ATENTADO Y RESISTENCIA- CABALLITOO165.docx.pdf</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>26  de  Agosto  del  2025</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>03:50  hs.-</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Atentado  y  Resistencia</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>45945869</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>Inspector  CISNEROS,  Pablo.  -</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>Oficial  Mayor  LEDESMA  Jesica</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>ZAMUDIO  Alejandro</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>UN  (01)  DETENIDO.  -</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>/Volumes/SIN NOMBRE/ultimo casi/PARTES/01DETENIDO-ROBO- MATADEROS12.docx.pdf</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>26  de  Agosto  del  2025</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>04:30hs.-</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>actuaciones  por  robo</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>45948394</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>Inspector  CISNEROS,  Pablo.  -</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>Oficial  LOPEZ  Maria</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>PINEL  Milagros</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>UN  (01)  DETENIDO  .  -</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>/Volumes/SIN NOMBRE/ultimo casi/PARTES/01DETENIDO-TTVA DE ROBO- CABALLITOO171.docx (3).pdf</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>26  de  Agosto  del  2025</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>01:35  hs.-</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Tentativa  de  Robo</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>45947733</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>Inspector  CISNEROS,  Pablo.  -</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>Oficial  Mayor  LEDESMA  Jesica</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>FEDELLE  Sandra</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>UN  (01)  DETENIDO.  -</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>/Volumes/SIN NOMBRE/ultimo casi/PARTES/2 CONTRAVENTORES- SAE 45941509.pdf</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>25 de Agosto del 2025</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>09:45</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>ARTICULO 239.</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>45941509</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>Oficial Mayor VERA, Erika.</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>Oficial Primero PERZ, Ramón</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>S/D</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>DOS (02) CONTRAVENTORES</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>/Volumes/SIN NOMBRE/ultimo casi/PARTES/02 DETENIDOS -AV. DE ILICITO- RECOLETA89.docx.pdf</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>26  de  Agosto  del  2025</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>01:17  hs.-</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>Averiguación  de  ilícito</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>45946858</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>Inspector  CISNEROS,  Pablo.  -</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>Oficial  Primero  MARTÍNEZ  Fernando</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>GONZALEZ,  Monica</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>DOS  (02)  DETENIDOS  .  -</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>/Volumes/SIN NOMBRE/ultimo casi/PARTES/02 IMPUTADOS-LEY23737- CONSTITUCION32.docx (1).pdf</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>25  de  Agosto  del  2025</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>21:00  hs.-</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>Ley  23.737</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>45945889</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>Inspector  CISNEROS,  Pablo.  -</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>Oficial  Primero  RIVERO  Marcos-</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>CASTILLO  Giselle</t>
+        </is>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>DOS  (02)  IMPURADOS  .  -</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>/Volumes/SIN NOMBRE/ultimo casi/PARTES/03IMPUTADOS-LEY23737- CONSTITUCION27.docx.pdf</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>26  de  Agosto  del  2025</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>04:30hs.-</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>ley  23737</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>45947743</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>Inspector  CISNEROS,  Pablo.  -</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>Oficial  Primero  RIVERO  Marcos</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>AQUINO  Juliana</t>
+        </is>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>TRES  (03)  IMPUTADOS  .  -</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>/Volumes/SIN NOMBRE/ultimo casi/PARTES/CABALLITOO134 - UN (01) DETENIDO.pdf</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>27 de agosto de 2025</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>03:04</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>ROBO</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>45956042</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>Inspector RODRIGUEZ Andres</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>Oficial CORTES Sebastian</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>Cont MENDOZ Luciano</t>
+        </is>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>UN (01) DETENIDO</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>/Volumes/SIN NOMBRE/ultimo casi/PARTES/CONSTITUCIÓNO139 - UN (01) DETENIDO.pdf</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>27 de agosto de 2025</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>01:49</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>15 de Noviembre de 1889 y Salta</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>45955883</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>Inspector RODRIGUEZ Andres</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>Oficial  CARABAJAL Graciela</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>Cont AQUINO Juliana</t>
+        </is>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>UN (01) DETENIDO</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>/Volumes/SIN NOMBRE/ultimo casi/PARTES/PALERMO 90 - UN (01)CONTRAVENTOR.pdf</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>26 de agosto de 2025</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>19:23</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>Av Santa Fe y Av Int Bullrich</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>45953934</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>Inspector RODRIGUEZ Andres</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>Oficial  COLO Nadia</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>Cont GONZALEZ Monica</t>
+        </is>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>UN (01) DETENIDO</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>/Volumes/SIN NOMBRE/ultimo casi/PARTES/PALERMOO175 - DOS (02) CONTRAVENTORES.pdf</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>26 de agosto de 2025</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>18:04</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>Av Infanta Isabel y Av del Libertador</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>45953383</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>Inspector RODRIGUEZ Andres</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>Oficial  COLO Nadia</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>Aux SEGOVIA Noelia</t>
+        </is>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>DOS (02) CONTRAVENTORES</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>/Volumes/SIN NOMBRE/ultimo casi/PARTES/VILLA LUGANO 61 - DOS (02) DETENIDOS.pdf</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>27 de agosto de 2025</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>01:46</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>AVERIGUACIÓN ILICITO</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>S/D</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>Inspector RODRIGUEZ Andres</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>Oficial  ALCARAZ Ariel</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>Cont ALDERETE Luciano</t>
+        </is>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>DOS (02) DETENIDOS</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>/Volumes/SIN NOMBRE/ultimo casi/PARTES/VILLA PUEYRREDÓN 59 - UN (01) DETENIDO.pdf</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>27 de agosto de 2025</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>03:51</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>TTVA ROBO</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>45956146</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>Inspector RODRIGUEZ Andres</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>Oficial COLO Nadia</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>Aux ROJAS Priscila</t>
+        </is>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>UN (01) DETENIDO</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
cambios en la grafica
</commit_message>
<xml_diff>
--- a/contenido_archivos.xlsx
+++ b/contenido_archivos.xlsx
@@ -430,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I52"/>
+  <dimension ref="A1:I64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2231,6 +2231,570 @@
       <c r="I52" t="inlineStr">
         <is>
           <t>UN (01) DETENIDO. –</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="2" t="inlineStr">
+        <is>
+          <t>/Users/alexisjankowicz/Downloads/01 DETENIDO-ART 104-  P PATRICIOS 41 .docx.pdf</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>28  de  agosto  de  2025</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>16:08</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>Art  104</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>45965420</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>Inspector  LP  4532  Aguirre  Alan</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>Oficial   lp  29049  Guzamn  Yesica</t>
+        </is>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>Personal  Contratado  Lamboglia  Lautaro</t>
+        </is>
+      </c>
+      <c r="I53" t="inlineStr">
+        <is>
+          <t>UN  (  1)DETENIDO</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="2" t="inlineStr">
+        <is>
+          <t>/Users/alexisjankowicz/Downloads/CABALLITOO109 - UN (01) DETENIDO.pdf</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>30 de agosto de 2025</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>03:29</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>ROBO</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>S/D</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>Inspector ARGUELLO Leandro</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>Oficial Primero ALCARAZ Ariel</t>
+        </is>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>Aux ROJAS Priscila</t>
+        </is>
+      </c>
+      <c r="I54" t="inlineStr">
+        <is>
+          <t>UN (01) DETENIDO</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="2" t="inlineStr">
+        <is>
+          <t>/Users/alexisjankowicz/Downloads/CONSTITUCIÓN11 - DOS (02) DETENIDOS.pdf</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>30 de agosto de 2025</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>03:48</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>ROBO</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>45981848</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>Inspector ARGUELLO Leandro</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>Oficial Primero ALCARAZ Ariel</t>
+        </is>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>Aux ROJAS Priscila</t>
+        </is>
+      </c>
+      <c r="I55" t="inlineStr">
+        <is>
+          <t>DOS (02) DETENIDOS</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="2" t="inlineStr">
+        <is>
+          <t>/Users/alexisjankowicz/Downloads/RECOLETAO115 - UN (01) DETENIDO.pdf</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>29 de agosto de 2025</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>23:28</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>AV INCENDIO</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>S/D</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>Inspector ARGUELLO Leandro</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>Oficial Primero VILLALBA Nicolas</t>
+        </is>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>Aux GARRIGO Agustina</t>
+        </is>
+      </c>
+      <c r="I56" t="inlineStr">
+        <is>
+          <t>UN (01) DETENIDO</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="2" t="inlineStr">
+        <is>
+          <t>/Users/alexisjankowicz/Downloads/SAN NICOLAS 67 - UN (01) DETENIDO.pdf</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>29 de agosto de 2025</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>22:01</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>TTVA HURTO</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>45979944</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>Inspector ARGUELLO Leandro</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>Inspector RODRIGUEZ Andres</t>
+        </is>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>Cont DONADON Nicolas</t>
+        </is>
+      </c>
+      <c r="I57" t="inlineStr">
+        <is>
+          <t>UN (01) DETENIDO</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="2" t="inlineStr">
+        <is>
+          <t>/Users/alexisjankowicz/Downloads/01 DETENIDO-ART 104-  P PATRICIOS 41 .docx.pdf</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>28  de  agosto  de  2025</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>16:08</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>Art  104</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>45965420</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>Inspector  LP  4532  Aguirre  Alan</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>Oficial   lp  29049  Guzamn  Yesica</t>
+        </is>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>Personal  Contratado  Lamboglia  Lautaro</t>
+        </is>
+      </c>
+      <c r="I58" t="inlineStr">
+        <is>
+          <t>UN  (  1)DETENIDO</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="2" t="inlineStr">
+        <is>
+          <t>/Users/alexisjankowicz/Downloads/CABALLITOO109 - UN (01) DETENIDO.pdf</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>30 de agosto de 2025</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>03:29</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>ROBO</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>S/D</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>Inspector ARGUELLO Leandro</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>Oficial Primero ALCARAZ Ariel</t>
+        </is>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>Aux ROJAS Priscila</t>
+        </is>
+      </c>
+      <c r="I59" t="inlineStr">
+        <is>
+          <t>UN (01) DETENIDO</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="2" t="inlineStr">
+        <is>
+          <t>/Users/alexisjankowicz/Downloads/CONSTITUCIÓN11 - DOS (02) DETENIDOS.pdf</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>30 de agosto de 2025</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>03:48</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>ROBO</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>45981848</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>Inspector ARGUELLO Leandro</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>Oficial Primero ALCARAZ Ariel</t>
+        </is>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>Aux ROJAS Priscila</t>
+        </is>
+      </c>
+      <c r="I60" t="inlineStr">
+        <is>
+          <t>DOS (02) DETENIDOS</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="2" t="inlineStr">
+        <is>
+          <t>/Users/alexisjankowicz/Downloads/RECOLETAO115 - UN (01) DETENIDO.pdf</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>29 de agosto de 2025</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>23:28</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>AV INCENDIO</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>S/D</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>Inspector ARGUELLO Leandro</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>Oficial Primero VILLALBA Nicolas</t>
+        </is>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>Aux GARRIGO Agustina</t>
+        </is>
+      </c>
+      <c r="I61" t="inlineStr">
+        <is>
+          <t>UN (01) DETENIDO</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="2" t="inlineStr">
+        <is>
+          <t>/Users/alexisjankowicz/Downloads/SAN NICOLAS 67 - UN (01) DETENIDO.pdf</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>29 de agosto de 2025</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>22:01</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>TTVA HURTO</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>45979944</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>Inspector ARGUELLO Leandro</t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>Inspector RODRIGUEZ Andres</t>
+        </is>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>Cont DONADON Nicolas</t>
+        </is>
+      </c>
+      <c r="I62" t="inlineStr">
+        <is>
+          <t>UN (01) DETENIDO</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="2" t="inlineStr">
+        <is>
+          <t>/Users/alexisjankowicz/Downloads/1 CONTRAVENTOR- SAE 45976643.pdf</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>29 de Agosto del 2025</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>17:00</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>ARTICULO 91 Y 239</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>45976643</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>Oficial Mayor MARTINEZ, Ricardo</t>
+        </is>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>Oficial PEREZ, Ramón</t>
+        </is>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>SEGOVIA, Noelia</t>
+        </is>
+      </c>
+      <c r="I63" t="inlineStr">
+        <is>
+          <t>UN (01) CONTRAVENTOR</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="2" t="inlineStr">
+        <is>
+          <t>/Users/alexisjankowicz/Downloads/CABALLITOO109 - UN (01) DETENIDO.pdf</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>30 de agosto de 2025</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>03:29</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>ROBO</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>S/D</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>Inspector ARGUELLO Leandro</t>
+        </is>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>Oficial Primero ALCARAZ Ariel</t>
+        </is>
+      </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>Aux ROJAS Priscila</t>
+        </is>
+      </c>
+      <c r="I64" t="inlineStr">
+        <is>
+          <t>UN (01) DETENIDO</t>
         </is>
       </c>
     </row>
@@ -2271,6 +2835,18 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A50" r:id="rId33"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A51" r:id="rId34"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A52" r:id="rId35"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A53" r:id="rId36"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A54" r:id="rId37"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A55" r:id="rId38"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A56" r:id="rId39"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A57" r:id="rId40"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A58" r:id="rId41"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A59" r:id="rId42"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A60" r:id="rId43"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A61" r:id="rId44"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A62" r:id="rId45"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A63" r:id="rId46"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A64" r:id="rId47"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>